<commit_message>
some work on new species
</commit_message>
<xml_diff>
--- a/data/ospree_searchers/baskinsearches_db.xlsx
+++ b/data/ospree_searchers/baskinsearches_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/egret/data/ospree_searchers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FEBB751-22C0-3A4A-8203-BB03739EA95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0336D835-2E55-3B4D-AD27-9BD95B6E4BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="760" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{889A57AF-BF39-5D40-9210-6ED7C554C77F}"/>
+    <workbookView xWindow="400" yWindow="1220" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{889A57AF-BF39-5D40-9210-6ED7C554C77F}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="82">
   <si>
     <t>genus</t>
   </si>
@@ -173,6 +173,114 @@
   </si>
   <si>
     <t>native vs. invasive comparison</t>
+  </si>
+  <si>
+    <t>Fraxinus</t>
+  </si>
+  <si>
+    <t>Steinbaur 1937</t>
+  </si>
+  <si>
+    <t>Bonner 1975</t>
+  </si>
+  <si>
+    <t>Villers &amp;Wareing 1964</t>
+  </si>
+  <si>
+    <t>Daleckaja et al 1970</t>
+  </si>
+  <si>
+    <t>Judin 1970</t>
+  </si>
+  <si>
+    <t>Rudinger and Dounavi 2008</t>
+  </si>
+  <si>
+    <t>Vandstone and LaCroix 1974</t>
+  </si>
+  <si>
+    <t>Benedict and David 2003</t>
+  </si>
+  <si>
+    <t>Arrigillia et al 1992</t>
+  </si>
+  <si>
+    <t>Piotto 1994</t>
+  </si>
+  <si>
+    <t>Cram &amp; Lindquist 1982</t>
+  </si>
+  <si>
+    <t>Fagus</t>
+  </si>
+  <si>
+    <t>Rudolf &amp; Leak 1974</t>
+  </si>
+  <si>
+    <t>Soltani et al 2005</t>
+  </si>
+  <si>
+    <t>Frankland &amp; Wareing 1966</t>
+  </si>
+  <si>
+    <t>Muller &amp; Laroppe 1993</t>
+  </si>
+  <si>
+    <t>Nowag 1998</t>
+  </si>
+  <si>
+    <t>Prochazkova &amp; Bezdeckova 2008,2009</t>
+  </si>
+  <si>
+    <t>Farmer &amp; Bonner 1967</t>
+  </si>
+  <si>
+    <t>McDermott 1953</t>
+  </si>
+  <si>
+    <t>Shirazi &amp; Ware 2003</t>
+  </si>
+  <si>
+    <t>Pence 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> not in umass library records https://agris.fao.org/search/en/providers/122607/records/6471f8082a40512c710f0c04</t>
+  </si>
+  <si>
+    <t>Not germination persay but something about embryo development</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Wcislinska 1977</t>
+  </si>
+  <si>
+    <t>5+</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>flooded vs unflood seeds was the treatment</t>
+  </si>
+  <si>
+    <t>propogration protocol</t>
+  </si>
+  <si>
+    <t>chemical and imbibation is the treatment</t>
+  </si>
+  <si>
+    <t>3?</t>
+  </si>
+  <si>
+    <t>not in Umass Library</t>
+  </si>
+  <si>
+    <t>Pyrus</t>
+  </si>
+  <si>
+    <t>Not in Baskin</t>
   </si>
 </sst>
 </file>
@@ -685,15 +793,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12744717-5B93-A544-A605-382F84106D6C}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" customWidth="1"/>
@@ -742,11 +852,8 @@
       <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
@@ -758,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
         <v>31</v>
@@ -774,32 +881,11 @@
       <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
       <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -813,33 +899,30 @@
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -848,33 +931,33 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -883,13 +966,13 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -898,13 +981,13 @@
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -914,32 +997,497 @@
       <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7">
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G11">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" t="s">
+        <v>78</v>
+      </c>
+      <c r="K22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>